<commit_message>
minor final version of day for version control
</commit_message>
<xml_diff>
--- a/mScThesis/twoTypeExcelfile.xlsx
+++ b/mScThesis/twoTypeExcelfile.xlsx
@@ -8,25 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MSc\Thesis\Simulation\C++\mScThesis\mScThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092C0135-2CFA-4CAE-9A87-AA67B2F4EE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAB1FD5-1072-435D-87A4-59D2B0A9D1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="20412" windowHeight="9132" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1341,11 +1330,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F276" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P302"/>
+    <sheetView tabSelected="1" topLeftCell="A283" workbookViewId="0">
+      <selection activeCell="M285" sqref="A1:P302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1432,7 +1424,7 @@
         <v>9.0500000000000007</v>
       </c>
       <c r="L2">
-        <v>7.4689285714285711</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="M2">
         <v>9.692678571428571</v>
@@ -1482,7 +1474,7 @@
         <v>16.850000000000001</v>
       </c>
       <c r="L3">
-        <v>22.360892857142851</v>
+        <v>16.850000000000001</v>
       </c>
       <c r="M3">
         <v>23.86964285714286</v>
@@ -1532,7 +1524,7 @@
         <v>15.2</v>
       </c>
       <c r="L4">
-        <v>18.891964285714291</v>
+        <v>15.2</v>
       </c>
       <c r="M4">
         <v>21.926964285714281</v>
@@ -1582,7 +1574,7 @@
         <v>13.25</v>
       </c>
       <c r="L5">
-        <v>8.3803571428571431</v>
+        <v>13.25</v>
       </c>
       <c r="M5">
         <v>11.01660714285714</v>
@@ -1632,7 +1624,7 @@
         <v>15</v>
       </c>
       <c r="L6">
-        <v>22.360892857142851</v>
+        <v>15</v>
       </c>
       <c r="M6">
         <v>23.86964285714286</v>
@@ -1682,7 +1674,7 @@
         <v>13</v>
       </c>
       <c r="L7">
-        <v>8.8360714285714295</v>
+        <v>13</v>
       </c>
       <c r="M7">
         <v>11.678571428571431</v>
@@ -1732,7 +1724,7 @@
         <v>18.45</v>
       </c>
       <c r="L8">
-        <v>20.655892857142859</v>
+        <v>18.45</v>
       </c>
       <c r="M8">
         <v>23.457142857142859</v>
@@ -1782,7 +1774,7 @@
         <v>8.75</v>
       </c>
       <c r="L9">
-        <v>18.436250000000001</v>
+        <v>8.75</v>
       </c>
       <c r="M9">
         <v>21.265000000000001</v>
@@ -1832,7 +1824,7 @@
         <v>10.65</v>
       </c>
       <c r="L10">
-        <v>17.980535714285711</v>
+        <v>10.65</v>
       </c>
       <c r="M10">
         <v>20.603035714285721</v>
@@ -1882,7 +1874,7 @@
         <v>16.95</v>
       </c>
       <c r="L11">
-        <v>18.891964285714291</v>
+        <v>16.95</v>
       </c>
       <c r="M11">
         <v>21.926964285714281</v>
@@ -1932,7 +1924,7 @@
         <v>12.95</v>
       </c>
       <c r="L12">
-        <v>19.28875</v>
+        <v>12.95</v>
       </c>
       <c r="M12">
         <v>22.32375</v>
@@ -1982,7 +1974,7 @@
         <v>12.05</v>
       </c>
       <c r="L13">
-        <v>23.21339285714286</v>
+        <v>12.05</v>
       </c>
       <c r="M13">
         <v>24.075892857142861</v>
@@ -2032,7 +2024,7 @@
         <v>9.4</v>
       </c>
       <c r="L14">
-        <v>22.360892857142851</v>
+        <v>9.4</v>
       </c>
       <c r="M14">
         <v>23.86964285714286</v>
@@ -2082,7 +2074,7 @@
         <v>11.2</v>
       </c>
       <c r="L15">
-        <v>21.508392857142859</v>
+        <v>11.2</v>
       </c>
       <c r="M15">
         <v>24.515892857142859</v>
@@ -2132,7 +2124,7 @@
         <v>17.7</v>
       </c>
       <c r="L16">
-        <v>19.34767857142857</v>
+        <v>17.7</v>
       </c>
       <c r="M16">
         <v>22.588928571428571</v>
@@ -2182,7 +2174,7 @@
         <v>12.05</v>
       </c>
       <c r="L17">
-        <v>23.21339285714286</v>
+        <v>12.05</v>
       </c>
       <c r="M17">
         <v>24.075892857142861</v>
@@ -2232,7 +2224,7 @@
         <v>8</v>
       </c>
       <c r="L18">
-        <v>7.8951785714285716</v>
+        <v>8</v>
       </c>
       <c r="M18">
         <v>10.32517857142857</v>
@@ -2282,7 +2274,7 @@
         <v>15.85</v>
       </c>
       <c r="L19">
-        <v>7.0132142857142856</v>
+        <v>15.85</v>
       </c>
       <c r="M19">
         <v>9.0307142857142857</v>
@@ -2332,7 +2324,7 @@
         <v>13.95</v>
       </c>
       <c r="L20">
-        <v>19.34767857142857</v>
+        <v>13.95</v>
       </c>
       <c r="M20">
         <v>22.588928571428571</v>
@@ -2382,7 +2374,7 @@
         <v>12.95</v>
       </c>
       <c r="L21">
-        <v>23.21339285714286</v>
+        <v>12.95</v>
       </c>
       <c r="M21">
         <v>24.075892857142861</v>
@@ -2432,7 +2424,7 @@
         <v>16.850000000000001</v>
       </c>
       <c r="L22">
-        <v>20.655892857142859</v>
+        <v>16.850000000000001</v>
       </c>
       <c r="M22">
         <v>23.457142857142859</v>
@@ -2482,7 +2474,7 @@
         <v>14</v>
       </c>
       <c r="L23">
-        <v>22.360892857142851</v>
+        <v>14</v>
       </c>
       <c r="M23">
         <v>23.86964285714286</v>
@@ -2532,7 +2524,7 @@
         <v>5</v>
       </c>
       <c r="L24">
-        <v>7.0132142857142856</v>
+        <v>18.149999999999999</v>
       </c>
       <c r="M24">
         <v>9.0307142857142857</v>
@@ -2582,7 +2574,7 @@
         <v>14.7</v>
       </c>
       <c r="L25">
-        <v>8.3803571428571431</v>
+        <v>14.7</v>
       </c>
       <c r="M25">
         <v>11.01660714285714</v>
@@ -2632,7 +2624,7 @@
         <v>5</v>
       </c>
       <c r="L26">
-        <v>17.980535714285711</v>
+        <v>5</v>
       </c>
       <c r="M26">
         <v>20.603035714285721</v>
@@ -2682,7 +2674,7 @@
         <v>9.4</v>
       </c>
       <c r="L27">
-        <v>19.80339285714286</v>
+        <v>9.4</v>
       </c>
       <c r="M27">
         <v>23.250892857142858</v>
@@ -2732,7 +2724,7 @@
         <v>10.3</v>
       </c>
       <c r="L28">
-        <v>7.9246428571428567</v>
+        <v>10.3</v>
       </c>
       <c r="M28">
         <v>10.35464285714286</v>
@@ -2782,7 +2774,7 @@
         <v>5</v>
       </c>
       <c r="L29">
-        <v>7.0132142857142856</v>
+        <v>16</v>
       </c>
       <c r="M29">
         <v>9.0307142857142857</v>
@@ -2832,7 +2824,7 @@
         <v>0</v>
       </c>
       <c r="L30">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M30">
         <v>2.4437500000000001</v>
@@ -2882,7 +2874,7 @@
         <v>10.5</v>
       </c>
       <c r="L31">
-        <v>22.360892857142851</v>
+        <v>10.5</v>
       </c>
       <c r="M31">
         <v>23.86964285714286</v>
@@ -2932,7 +2924,7 @@
         <v>12.8</v>
       </c>
       <c r="L32">
-        <v>7.9246428571428567</v>
+        <v>12.8</v>
       </c>
       <c r="M32">
         <v>10.35464285714286</v>
@@ -2982,7 +2974,7 @@
         <v>6.05</v>
       </c>
       <c r="L33">
-        <v>7.9246428571428567</v>
+        <v>6.05</v>
       </c>
       <c r="M33">
         <v>10.35464285714286</v>
@@ -3032,7 +3024,7 @@
         <v>8</v>
       </c>
       <c r="L34">
-        <v>7.4689285714285711</v>
+        <v>8</v>
       </c>
       <c r="M34">
         <v>9.692678571428571</v>
@@ -3082,7 +3074,7 @@
         <v>11.45</v>
       </c>
       <c r="L35">
-        <v>8.3803571428571431</v>
+        <v>11.45</v>
       </c>
       <c r="M35">
         <v>11.01660714285714</v>
@@ -3132,7 +3124,7 @@
         <v>7.7</v>
       </c>
       <c r="L36">
-        <v>8.3803571428571431</v>
+        <v>7.7</v>
       </c>
       <c r="M36">
         <v>11.01660714285714</v>
@@ -3182,7 +3174,7 @@
         <v>4</v>
       </c>
       <c r="L37">
-        <v>8.3508928571428562</v>
+        <v>4</v>
       </c>
       <c r="M37">
         <v>10.98714285714286</v>
@@ -3232,7 +3224,7 @@
         <v>11.1</v>
       </c>
       <c r="L38">
-        <v>17.980535714285711</v>
+        <v>11.1</v>
       </c>
       <c r="M38">
         <v>20.603035714285721</v>
@@ -3282,7 +3274,7 @@
         <v>6</v>
       </c>
       <c r="L39">
-        <v>7.9246428571428567</v>
+        <v>6</v>
       </c>
       <c r="M39">
         <v>10.35464285714286</v>
@@ -3332,7 +3324,7 @@
         <v>4</v>
       </c>
       <c r="L40">
-        <v>22.360892857142851</v>
+        <v>4</v>
       </c>
       <c r="M40">
         <v>23.86964285714286</v>
@@ -3382,7 +3374,7 @@
         <v>9.25</v>
       </c>
       <c r="L41">
-        <v>19.80339285714286</v>
+        <v>9.25</v>
       </c>
       <c r="M41">
         <v>23.250892857142858</v>
@@ -3432,7 +3424,7 @@
         <v>14</v>
       </c>
       <c r="L42">
-        <v>18.891964285714291</v>
+        <v>14</v>
       </c>
       <c r="M42">
         <v>21.926964285714281</v>
@@ -3482,7 +3474,7 @@
         <v>9.1</v>
       </c>
       <c r="L43">
-        <v>19.34767857142857</v>
+        <v>9.1</v>
       </c>
       <c r="M43">
         <v>22.588928571428571</v>
@@ -3532,7 +3524,7 @@
         <v>10.45</v>
       </c>
       <c r="L44">
-        <v>23.21339285714286</v>
+        <v>10.45</v>
       </c>
       <c r="M44">
         <v>24.075892857142861</v>
@@ -3582,7 +3574,7 @@
         <v>12.2</v>
       </c>
       <c r="L45">
-        <v>21.508392857142859</v>
+        <v>12.2</v>
       </c>
       <c r="M45">
         <v>23.66339285714286</v>
@@ -3632,7 +3624,7 @@
         <v>14.2</v>
       </c>
       <c r="L46">
-        <v>20.993749999999999</v>
+        <v>14.2</v>
       </c>
       <c r="M46">
         <v>24.44125</v>
@@ -3682,7 +3674,7 @@
         <v>12.6</v>
       </c>
       <c r="L47">
-        <v>19.80339285714286</v>
+        <v>12.6</v>
       </c>
       <c r="M47">
         <v>23.250892857142858</v>
@@ -3732,7 +3724,7 @@
         <v>10.9</v>
       </c>
       <c r="L48">
-        <v>23.21339285714286</v>
+        <v>10.9</v>
       </c>
       <c r="M48">
         <v>24.075892857142861</v>
@@ -3782,7 +3774,7 @@
         <v>8.75</v>
       </c>
       <c r="L49">
-        <v>18.436250000000001</v>
+        <v>8.75</v>
       </c>
       <c r="M49">
         <v>21.265000000000001</v>
@@ -3832,7 +3824,7 @@
         <v>16.850000000000001</v>
       </c>
       <c r="L50">
-        <v>22.360892857142851</v>
+        <v>16.850000000000001</v>
       </c>
       <c r="M50">
         <v>23.86964285714286</v>
@@ -3882,7 +3874,7 @@
         <v>13.2</v>
       </c>
       <c r="L51">
-        <v>19.34767857142857</v>
+        <v>13.2</v>
       </c>
       <c r="M51">
         <v>22.588928571428571</v>
@@ -3932,7 +3924,7 @@
         <v>10.050000000000001</v>
       </c>
       <c r="L52">
-        <v>17.980535714285711</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="M52">
         <v>20.603035714285721</v>
@@ -3982,7 +3974,7 @@
         <v>11.1</v>
       </c>
       <c r="L53">
-        <v>20.655892857142859</v>
+        <v>11.1</v>
       </c>
       <c r="M53">
         <v>23.457142857142859</v>
@@ -4032,7 +4024,7 @@
         <v>11.4</v>
       </c>
       <c r="L54">
-        <v>17.980535714285711</v>
+        <v>11.4</v>
       </c>
       <c r="M54">
         <v>20.603035714285721</v>
@@ -4082,7 +4074,7 @@
         <v>11.7</v>
       </c>
       <c r="L55">
-        <v>18.891964285714291</v>
+        <v>11.7</v>
       </c>
       <c r="M55">
         <v>21.926964285714281</v>
@@ -4132,7 +4124,7 @@
         <v>5</v>
       </c>
       <c r="L56">
-        <v>21.508392857142859</v>
+        <v>5</v>
       </c>
       <c r="M56">
         <v>23.66339285714286</v>
@@ -4182,7 +4174,7 @@
         <v>6</v>
       </c>
       <c r="L57">
-        <v>18.891964285714291</v>
+        <v>6</v>
       </c>
       <c r="M57">
         <v>21.926964285714281</v>
@@ -4232,7 +4224,7 @@
         <v>13.35</v>
       </c>
       <c r="L58">
-        <v>22.360892857142851</v>
+        <v>13.35</v>
       </c>
       <c r="M58">
         <v>23.86964285714286</v>
@@ -4282,7 +4274,7 @@
         <v>11.1</v>
       </c>
       <c r="L59">
-        <v>8.3803571428571431</v>
+        <v>11.1</v>
       </c>
       <c r="M59">
         <v>11.01660714285714</v>
@@ -4332,7 +4324,7 @@
         <v>13.95</v>
       </c>
       <c r="L60">
-        <v>22.360892857142851</v>
+        <v>13.95</v>
       </c>
       <c r="M60">
         <v>23.86964285714286</v>
@@ -4382,7 +4374,7 @@
         <v>11.45</v>
       </c>
       <c r="L61">
-        <v>19.80339285714286</v>
+        <v>11.45</v>
       </c>
       <c r="M61">
         <v>23.250892857142858</v>
@@ -4432,7 +4424,7 @@
         <v>11.4</v>
       </c>
       <c r="L62">
-        <v>20.655892857142859</v>
+        <v>11.4</v>
       </c>
       <c r="M62">
         <v>23.457142857142859</v>
@@ -4482,7 +4474,7 @@
         <v>5</v>
       </c>
       <c r="L63">
-        <v>23.21339285714286</v>
+        <v>5</v>
       </c>
       <c r="M63">
         <v>24.075892857142861</v>
@@ -4532,7 +4524,7 @@
         <v>9.5</v>
       </c>
       <c r="L64">
-        <v>24.006964285714279</v>
+        <v>9.5</v>
       </c>
       <c r="M64">
         <v>28.27946428571429</v>
@@ -4582,7 +4574,7 @@
         <v>9.25</v>
       </c>
       <c r="L65">
-        <v>9.1444642857142853</v>
+        <v>9.25</v>
       </c>
       <c r="M65">
         <v>12.193214285714291</v>
@@ -4632,7 +4624,7 @@
         <v>11.95</v>
       </c>
       <c r="L66">
-        <v>18.891964285714291</v>
+        <v>11.95</v>
       </c>
       <c r="M66">
         <v>21.926964285714281</v>
@@ -4682,7 +4674,7 @@
         <v>8.0500000000000007</v>
       </c>
       <c r="L67">
-        <v>8.8360714285714295</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="M67">
         <v>11.678571428571431</v>
@@ -4732,7 +4724,7 @@
         <v>9.75</v>
       </c>
       <c r="L68">
-        <v>7.9246428571428567</v>
+        <v>9.75</v>
       </c>
       <c r="M68">
         <v>10.35464285714286</v>
@@ -4782,7 +4774,7 @@
         <v>14.3</v>
       </c>
       <c r="L69">
-        <v>19.80339285714286</v>
+        <v>14.3</v>
       </c>
       <c r="M69">
         <v>23.250892857142858</v>
@@ -4832,7 +4824,7 @@
         <v>12.05</v>
       </c>
       <c r="L70">
-        <v>18.436250000000001</v>
+        <v>12.05</v>
       </c>
       <c r="M70">
         <v>21.265000000000001</v>
@@ -4882,7 +4874,7 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="L71">
-        <v>7.0132142857142856</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="M71">
         <v>9.0307142857142857</v>
@@ -4932,7 +4924,7 @@
         <v>0</v>
       </c>
       <c r="L72">
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="M72">
         <v>2.2374999999999998</v>
@@ -4982,7 +4974,7 @@
         <v>10.45</v>
       </c>
       <c r="L73">
-        <v>20.655892857142859</v>
+        <v>10.45</v>
       </c>
       <c r="M73">
         <v>23.457142857142859</v>
@@ -5032,7 +5024,7 @@
         <v>11.8</v>
       </c>
       <c r="L74">
-        <v>19.80339285714286</v>
+        <v>11.8</v>
       </c>
       <c r="M74">
         <v>23.250892857142858</v>
@@ -5082,7 +5074,7 @@
         <v>6</v>
       </c>
       <c r="L75">
-        <v>17.980535714285711</v>
+        <v>6</v>
       </c>
       <c r="M75">
         <v>20.603035714285721</v>
@@ -5132,7 +5124,7 @@
         <v>9.75</v>
       </c>
       <c r="L76">
-        <v>8.3803571428571431</v>
+        <v>9.75</v>
       </c>
       <c r="M76">
         <v>11.01660714285714</v>
@@ -5182,7 +5174,7 @@
         <v>12.15</v>
       </c>
       <c r="L77">
-        <v>8.8360714285714295</v>
+        <v>12.15</v>
       </c>
       <c r="M77">
         <v>11.678571428571431</v>
@@ -5232,7 +5224,7 @@
         <v>11.9</v>
       </c>
       <c r="L78">
-        <v>23.21339285714286</v>
+        <v>11.9</v>
       </c>
       <c r="M78">
         <v>24.075892857142861</v>
@@ -5282,7 +5274,7 @@
         <v>7.75</v>
       </c>
       <c r="L79">
-        <v>21.508392857142859</v>
+        <v>7.75</v>
       </c>
       <c r="M79">
         <v>23.66339285714286</v>
@@ -5332,7 +5324,7 @@
         <v>8.35</v>
       </c>
       <c r="L80">
-        <v>7.0132142857142856</v>
+        <v>8.35</v>
       </c>
       <c r="M80">
         <v>9.0307142857142857</v>
@@ -5382,7 +5374,7 @@
         <v>12.1</v>
       </c>
       <c r="L81">
-        <v>17.980535714285711</v>
+        <v>12.1</v>
       </c>
       <c r="M81">
         <v>20.603035714285721</v>
@@ -5432,7 +5424,7 @@
         <v>6</v>
       </c>
       <c r="L82">
-        <v>20.655892857142859</v>
+        <v>6</v>
       </c>
       <c r="M82">
         <v>23.457142857142859</v>
@@ -5482,7 +5474,7 @@
         <v>10.45</v>
       </c>
       <c r="L83">
-        <v>18.891964285714291</v>
+        <v>10.45</v>
       </c>
       <c r="M83">
         <v>21.926964285714281</v>
@@ -5532,7 +5524,7 @@
         <v>10.5</v>
       </c>
       <c r="L84">
-        <v>19.28875</v>
+        <v>10.5</v>
       </c>
       <c r="M84">
         <v>22.32375</v>
@@ -5582,7 +5574,7 @@
         <v>0</v>
       </c>
       <c r="L85">
-        <v>0</v>
+        <v>6.4</v>
       </c>
       <c r="M85">
         <v>2.2374999999999998</v>
@@ -5632,7 +5624,7 @@
         <v>6</v>
       </c>
       <c r="L86">
-        <v>19.80339285714286</v>
+        <v>6</v>
       </c>
       <c r="M86">
         <v>23.250892857142858</v>
@@ -5682,7 +5674,7 @@
         <v>0</v>
       </c>
       <c r="L87">
-        <v>0</v>
+        <v>13.65</v>
       </c>
       <c r="M87">
         <v>2.2374999999999998</v>
@@ -5732,7 +5724,7 @@
         <v>10.1</v>
       </c>
       <c r="L88">
-        <v>18.436250000000001</v>
+        <v>10.1</v>
       </c>
       <c r="M88">
         <v>21.265000000000001</v>
@@ -5782,7 +5774,7 @@
         <v>10.45</v>
       </c>
       <c r="L89">
-        <v>20.655892857142859</v>
+        <v>10.45</v>
       </c>
       <c r="M89">
         <v>23.457142857142859</v>
@@ -5832,7 +5824,7 @@
         <v>11.6</v>
       </c>
       <c r="L90">
-        <v>19.80339285714286</v>
+        <v>11.6</v>
       </c>
       <c r="M90">
         <v>23.250892857142858</v>
@@ -5882,7 +5874,7 @@
         <v>10.1</v>
       </c>
       <c r="L91">
-        <v>18.891964285714291</v>
+        <v>10.1</v>
       </c>
       <c r="M91">
         <v>21.926964285714281</v>
@@ -5932,7 +5924,7 @@
         <v>6</v>
       </c>
       <c r="L92">
-        <v>7.0132142857142856</v>
+        <v>6</v>
       </c>
       <c r="M92">
         <v>9.0307142857142857</v>
@@ -5982,7 +5974,7 @@
         <v>13.55</v>
       </c>
       <c r="L93">
-        <v>20.655892857142859</v>
+        <v>13.55</v>
       </c>
       <c r="M93">
         <v>23.457142857142859</v>
@@ -6032,7 +6024,7 @@
         <v>0</v>
       </c>
       <c r="L94">
-        <v>0</v>
+        <v>13.3</v>
       </c>
       <c r="M94">
         <v>2.2374999999999998</v>
@@ -6082,7 +6074,7 @@
         <v>10.1</v>
       </c>
       <c r="L95">
-        <v>7.0132142857142856</v>
+        <v>10.1</v>
       </c>
       <c r="M95">
         <v>9.0307142857142857</v>
@@ -6132,7 +6124,7 @@
         <v>5</v>
       </c>
       <c r="L96">
-        <v>8.3803571428571431</v>
+        <v>5</v>
       </c>
       <c r="M96">
         <v>11.01660714285714</v>
@@ -6182,7 +6174,7 @@
         <v>8</v>
       </c>
       <c r="L97">
-        <v>7.0132142857142856</v>
+        <v>8</v>
       </c>
       <c r="M97">
         <v>9.0307142857142857</v>
@@ -6232,7 +6224,7 @@
         <v>16.75</v>
       </c>
       <c r="L98">
-        <v>20.655892857142859</v>
+        <v>16.75</v>
       </c>
       <c r="M98">
         <v>23.457142857142859</v>
@@ -6282,7 +6274,7 @@
         <v>11.95</v>
       </c>
       <c r="L99">
-        <v>21.508392857142859</v>
+        <v>11.95</v>
       </c>
       <c r="M99">
         <v>23.66339285714286</v>
@@ -6332,7 +6324,7 @@
         <v>7</v>
       </c>
       <c r="L100">
-        <v>18.891964285714291</v>
+        <v>7</v>
       </c>
       <c r="M100">
         <v>21.926964285714281</v>
@@ -6382,7 +6374,7 @@
         <v>7</v>
       </c>
       <c r="L101">
-        <v>18.891964285714291</v>
+        <v>7</v>
       </c>
       <c r="M101">
         <v>21.926964285714281</v>
@@ -6432,7 +6424,7 @@
         <v>0</v>
       </c>
       <c r="L102">
-        <v>0</v>
+        <v>10.6</v>
       </c>
       <c r="M102">
         <v>2.2374999999999998</v>
@@ -6482,7 +6474,7 @@
         <v>9.75</v>
       </c>
       <c r="L103">
-        <v>7.4394642857142852</v>
+        <v>9.75</v>
       </c>
       <c r="M103">
         <v>9.663214285714286</v>
@@ -6532,7 +6524,7 @@
         <v>8.0500000000000007</v>
       </c>
       <c r="L104">
-        <v>19.34767857142857</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="M104">
         <v>22.588928571428571</v>
@@ -6582,7 +6574,7 @@
         <v>8</v>
       </c>
       <c r="L105">
-        <v>9.2328571428571422</v>
+        <v>8</v>
       </c>
       <c r="M105">
         <v>12.281607142857141</v>
@@ -6632,7 +6624,7 @@
         <v>0</v>
       </c>
       <c r="L106">
-        <v>0</v>
+        <v>12.85</v>
       </c>
       <c r="M106">
         <v>2.2374999999999998</v>
@@ -6682,7 +6674,7 @@
         <v>11.7</v>
       </c>
       <c r="L107">
-        <v>19.34767857142857</v>
+        <v>11.7</v>
       </c>
       <c r="M107">
         <v>22.588928571428571</v>
@@ -6732,7 +6724,7 @@
         <v>7.7</v>
       </c>
       <c r="L108">
-        <v>7.0132142857142856</v>
+        <v>7.7</v>
       </c>
       <c r="M108">
         <v>9.0307142857142857</v>
@@ -6782,7 +6774,7 @@
         <v>9</v>
       </c>
       <c r="L109">
-        <v>23.21339285714286</v>
+        <v>9</v>
       </c>
       <c r="M109">
         <v>24.075892857142861</v>
@@ -6832,7 +6824,7 @@
         <v>12.5</v>
       </c>
       <c r="L110">
-        <v>23.21339285714286</v>
+        <v>12.5</v>
       </c>
       <c r="M110">
         <v>24.075892857142861</v>
@@ -6882,7 +6874,7 @@
         <v>15.9</v>
       </c>
       <c r="L111">
-        <v>8.3803571428571431</v>
+        <v>15.9</v>
       </c>
       <c r="M111">
         <v>11.01660714285714</v>
@@ -6932,7 +6924,7 @@
         <v>12.65</v>
       </c>
       <c r="L112">
-        <v>19.80339285714286</v>
+        <v>12.65</v>
       </c>
       <c r="M112">
         <v>23.250892857142858</v>
@@ -6982,7 +6974,7 @@
         <v>15</v>
       </c>
       <c r="L113">
-        <v>21.508392857142859</v>
+        <v>15</v>
       </c>
       <c r="M113">
         <v>23.66339285714286</v>
@@ -7032,7 +7024,7 @@
         <v>10.1</v>
       </c>
       <c r="L114">
-        <v>7.0132142857142856</v>
+        <v>10.1</v>
       </c>
       <c r="M114">
         <v>9.0307142857142857</v>
@@ -7082,7 +7074,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="L115">
-        <v>7.4689285714285711</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="M115">
         <v>9.692678571428571</v>
@@ -7132,7 +7124,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="L116">
-        <v>8.3803571428571431</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="M116">
         <v>11.01660714285714</v>
@@ -7182,7 +7174,7 @@
         <v>14.95</v>
       </c>
       <c r="L117">
-        <v>18.891964285714291</v>
+        <v>14.95</v>
       </c>
       <c r="M117">
         <v>21.926964285714281</v>
@@ -7232,7 +7224,7 @@
         <v>9.5</v>
       </c>
       <c r="L118">
-        <v>7.0132142857142856</v>
+        <v>9.5</v>
       </c>
       <c r="M118">
         <v>9.0307142857142857</v>
@@ -7282,7 +7274,7 @@
         <v>8.85</v>
       </c>
       <c r="L119">
-        <v>8.3803571428571431</v>
+        <v>8.85</v>
       </c>
       <c r="M119">
         <v>11.01660714285714</v>
@@ -7332,7 +7324,7 @@
         <v>9.25</v>
       </c>
       <c r="L120">
-        <v>19.80339285714286</v>
+        <v>9.25</v>
       </c>
       <c r="M120">
         <v>23.250892857142858</v>
@@ -7382,7 +7374,7 @@
         <v>12.2</v>
       </c>
       <c r="L121">
-        <v>20.655892857142859</v>
+        <v>12.2</v>
       </c>
       <c r="M121">
         <v>23.457142857142859</v>
@@ -7432,7 +7424,7 @@
         <v>10.45</v>
       </c>
       <c r="L122">
-        <v>21.508392857142859</v>
+        <v>10.45</v>
       </c>
       <c r="M122">
         <v>23.66339285714286</v>
@@ -7482,7 +7474,7 @@
         <v>11.9</v>
       </c>
       <c r="L123">
-        <v>7.4689285714285711</v>
+        <v>11.9</v>
       </c>
       <c r="M123">
         <v>9.692678571428571</v>
@@ -7532,7 +7524,7 @@
         <v>10.5</v>
       </c>
       <c r="L124">
-        <v>20.655892857142859</v>
+        <v>10.5</v>
       </c>
       <c r="M124">
         <v>23.457142857142859</v>
@@ -7582,7 +7574,7 @@
         <v>7.35</v>
       </c>
       <c r="L125">
-        <v>20.596964285714289</v>
+        <v>7.35</v>
       </c>
       <c r="M125">
         <v>24.044464285714291</v>
@@ -7632,7 +7624,7 @@
         <v>10.35</v>
       </c>
       <c r="L126">
-        <v>7.9246428571428567</v>
+        <v>10.35</v>
       </c>
       <c r="M126">
         <v>10.35464285714286</v>
@@ -7682,7 +7674,7 @@
         <v>10</v>
       </c>
       <c r="L127">
-        <v>8.8360714285714295</v>
+        <v>10</v>
       </c>
       <c r="M127">
         <v>11.678571428571431</v>
@@ -7732,7 +7724,7 @@
         <v>12.55</v>
       </c>
       <c r="L128">
-        <v>22.360892857142851</v>
+        <v>12.55</v>
       </c>
       <c r="M128">
         <v>23.86964285714286</v>
@@ -7782,7 +7774,7 @@
         <v>7</v>
       </c>
       <c r="L129">
-        <v>19.80339285714286</v>
+        <v>7</v>
       </c>
       <c r="M129">
         <v>23.250892857142858</v>
@@ -7832,7 +7824,7 @@
         <v>8.35</v>
       </c>
       <c r="L130">
-        <v>23.21339285714286</v>
+        <v>8.35</v>
       </c>
       <c r="M130">
         <v>24.92839285714286</v>
@@ -7882,7 +7874,7 @@
         <v>10.5</v>
       </c>
       <c r="L131">
-        <v>7.0132142857142856</v>
+        <v>10.5</v>
       </c>
       <c r="M131">
         <v>9.0307142857142857</v>
@@ -7932,7 +7924,7 @@
         <v>12.65</v>
       </c>
       <c r="L132">
-        <v>7.9246428571428567</v>
+        <v>12.65</v>
       </c>
       <c r="M132">
         <v>10.35464285714286</v>
@@ -7982,7 +7974,7 @@
         <v>8.4</v>
       </c>
       <c r="L133">
-        <v>18.436250000000001</v>
+        <v>8.4</v>
       </c>
       <c r="M133">
         <v>21.265000000000001</v>
@@ -8032,7 +8024,7 @@
         <v>8.25</v>
       </c>
       <c r="L134">
-        <v>20.655892857142859</v>
+        <v>8.25</v>
       </c>
       <c r="M134">
         <v>23.457142857142859</v>
@@ -8082,7 +8074,7 @@
         <v>7.75</v>
       </c>
       <c r="L135">
-        <v>21.508392857142859</v>
+        <v>7.75</v>
       </c>
       <c r="M135">
         <v>23.66339285714286</v>
@@ -8132,7 +8124,7 @@
         <v>12.9</v>
       </c>
       <c r="L136">
-        <v>18.436250000000001</v>
+        <v>12.9</v>
       </c>
       <c r="M136">
         <v>21.265000000000001</v>
@@ -8182,7 +8174,7 @@
         <v>11.5</v>
       </c>
       <c r="L137">
-        <v>18.436250000000001</v>
+        <v>11.5</v>
       </c>
       <c r="M137">
         <v>21.265000000000001</v>
@@ -8232,7 +8224,7 @@
         <v>13.5</v>
       </c>
       <c r="L138">
-        <v>7.0132142857142856</v>
+        <v>13.5</v>
       </c>
       <c r="M138">
         <v>9.0307142857142857</v>
@@ -8282,7 +8274,7 @@
         <v>6.4</v>
       </c>
       <c r="L139">
-        <v>8.3803571428571431</v>
+        <v>6.4</v>
       </c>
       <c r="M139">
         <v>11.01660714285714</v>
@@ -8332,7 +8324,7 @@
         <v>7.25</v>
       </c>
       <c r="L140">
-        <v>8.3508928571428562</v>
+        <v>7.25</v>
       </c>
       <c r="M140">
         <v>10.98714285714286</v>
@@ -8382,7 +8374,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="L141">
-        <v>20.596964285714289</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="M141">
         <v>24.044464285714291</v>
@@ -8432,7 +8424,7 @@
         <v>13.7</v>
       </c>
       <c r="L142">
-        <v>19.74446428571429</v>
+        <v>13.7</v>
       </c>
       <c r="M142">
         <v>22.985714285714291</v>
@@ -8482,7 +8474,7 @@
         <v>10.25</v>
       </c>
       <c r="L143">
-        <v>18.891964285714291</v>
+        <v>10.25</v>
       </c>
       <c r="M143">
         <v>21.926964285714281</v>
@@ -8532,7 +8524,7 @@
         <v>12.55</v>
       </c>
       <c r="L144">
-        <v>8.3803571428571431</v>
+        <v>12.55</v>
       </c>
       <c r="M144">
         <v>11.01660714285714</v>
@@ -8582,7 +8574,7 @@
         <v>5</v>
       </c>
       <c r="L145">
-        <v>19.80339285714286</v>
+        <v>5</v>
       </c>
       <c r="M145">
         <v>23.250892857142858</v>
@@ -8632,7 +8624,7 @@
         <v>15.35</v>
       </c>
       <c r="L146">
-        <v>7.9246428571428567</v>
+        <v>15.35</v>
       </c>
       <c r="M146">
         <v>10.35464285714286</v>
@@ -8682,7 +8674,7 @@
         <v>11.85</v>
       </c>
       <c r="L147">
-        <v>17.980535714285711</v>
+        <v>11.85</v>
       </c>
       <c r="M147">
         <v>20.603035714285721</v>
@@ -8732,7 +8724,7 @@
         <v>11</v>
       </c>
       <c r="L148">
-        <v>23.21339285714286</v>
+        <v>11</v>
       </c>
       <c r="M148">
         <v>24.075892857142861</v>
@@ -8782,7 +8774,7 @@
         <v>9.1</v>
       </c>
       <c r="L149">
-        <v>8.8360714285714295</v>
+        <v>9.1</v>
       </c>
       <c r="M149">
         <v>11.678571428571431</v>
@@ -8832,7 +8824,7 @@
         <v>17.25</v>
       </c>
       <c r="L150">
-        <v>20.655892857142859</v>
+        <v>17.25</v>
       </c>
       <c r="M150">
         <v>24.309642857142862</v>
@@ -8882,7 +8874,7 @@
         <v>15.6</v>
       </c>
       <c r="L151">
-        <v>19.685535714285709</v>
+        <v>15.6</v>
       </c>
       <c r="M151">
         <v>22.72053571428571</v>
@@ -8932,7 +8924,7 @@
         <v>15.7</v>
       </c>
       <c r="L152">
-        <v>17.980535714285711</v>
+        <v>15.7</v>
       </c>
       <c r="M152">
         <v>20.603035714285721</v>
@@ -8982,7 +8974,7 @@
         <v>14.6</v>
       </c>
       <c r="L153">
-        <v>21.508392857142859</v>
+        <v>14.6</v>
       </c>
       <c r="M153">
         <v>23.66339285714286</v>
@@ -9032,7 +9024,7 @@
         <v>0</v>
       </c>
       <c r="L154">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="M154">
         <v>2.2374999999999998</v>
@@ -9082,7 +9074,7 @@
         <v>14.1</v>
       </c>
       <c r="L155">
-        <v>18.891964285714291</v>
+        <v>14.1</v>
       </c>
       <c r="M155">
         <v>21.926964285714281</v>
@@ -9132,7 +9124,7 @@
         <v>3</v>
       </c>
       <c r="L156">
-        <v>22.360892857142851</v>
+        <v>3</v>
       </c>
       <c r="M156">
         <v>23.86964285714286</v>
@@ -9182,7 +9174,7 @@
         <v>3</v>
       </c>
       <c r="L157">
-        <v>22.360892857142851</v>
+        <v>3</v>
       </c>
       <c r="M157">
         <v>23.86964285714286</v>
@@ -9232,7 +9224,7 @@
         <v>14.55</v>
       </c>
       <c r="L158">
-        <v>7.0132142857142856</v>
+        <v>14.55</v>
       </c>
       <c r="M158">
         <v>9.0307142857142857</v>
@@ -9282,7 +9274,7 @@
         <v>12.35</v>
       </c>
       <c r="L159">
-        <v>19.80339285714286</v>
+        <v>12.35</v>
       </c>
       <c r="M159">
         <v>23.250892857142858</v>
@@ -9332,7 +9324,7 @@
         <v>8.5</v>
       </c>
       <c r="L160">
-        <v>23.21339285714286</v>
+        <v>8.5</v>
       </c>
       <c r="M160">
         <v>24.075892857142861</v>
@@ -9382,7 +9374,7 @@
         <v>0</v>
       </c>
       <c r="L161">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M161">
         <v>2.2374999999999998</v>
@@ -9432,7 +9424,7 @@
         <v>0</v>
       </c>
       <c r="L162">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M162">
         <v>2.2374999999999998</v>
@@ -9482,7 +9474,7 @@
         <v>6</v>
       </c>
       <c r="L163">
-        <v>8.3803571428571431</v>
+        <v>6</v>
       </c>
       <c r="M163">
         <v>11.01660714285714</v>
@@ -9532,7 +9524,7 @@
         <v>10.15</v>
       </c>
       <c r="L164">
-        <v>20.655892857142859</v>
+        <v>10.15</v>
       </c>
       <c r="M164">
         <v>24.309642857142862</v>
@@ -9582,7 +9574,7 @@
         <v>12.2</v>
       </c>
       <c r="L165">
-        <v>7.0132142857142856</v>
+        <v>12.2</v>
       </c>
       <c r="M165">
         <v>9.0307142857142857</v>
@@ -9632,7 +9624,7 @@
         <v>18.2</v>
       </c>
       <c r="L166">
-        <v>19.34767857142857</v>
+        <v>18.2</v>
       </c>
       <c r="M166">
         <v>22.588928571428571</v>
@@ -9682,7 +9674,7 @@
         <v>11.55</v>
       </c>
       <c r="L167">
-        <v>18.83303571428571</v>
+        <v>11.55</v>
       </c>
       <c r="M167">
         <v>21.66178571428571</v>
@@ -9732,7 +9724,7 @@
         <v>15.1</v>
       </c>
       <c r="L168">
-        <v>18.436250000000001</v>
+        <v>15.1</v>
       </c>
       <c r="M168">
         <v>21.265000000000001</v>
@@ -9782,7 +9774,7 @@
         <v>12.25</v>
       </c>
       <c r="L169">
-        <v>8.3508928571428562</v>
+        <v>12.25</v>
       </c>
       <c r="M169">
         <v>10.98714285714286</v>
@@ -9832,7 +9824,7 @@
         <v>10</v>
       </c>
       <c r="L170">
-        <v>19.80339285714286</v>
+        <v>10</v>
       </c>
       <c r="M170">
         <v>23.250892857142858</v>
@@ -9882,7 +9874,7 @@
         <v>12</v>
       </c>
       <c r="L171">
-        <v>19.80339285714286</v>
+        <v>12</v>
       </c>
       <c r="M171">
         <v>23.250892857142858</v>
@@ -9932,7 +9924,7 @@
         <v>10.75</v>
       </c>
       <c r="L172">
-        <v>18.891964285714291</v>
+        <v>10.75</v>
       </c>
       <c r="M172">
         <v>21.926964285714281</v>
@@ -9982,7 +9974,7 @@
         <v>9.1</v>
       </c>
       <c r="L173">
-        <v>7.9246428571428567</v>
+        <v>9.1</v>
       </c>
       <c r="M173">
         <v>10.35464285714286</v>
@@ -10032,7 +10024,7 @@
         <v>17.45</v>
       </c>
       <c r="L174">
-        <v>23.21339285714286</v>
+        <v>17.45</v>
       </c>
       <c r="M174">
         <v>24.075892857142861</v>
@@ -10082,7 +10074,7 @@
         <v>13.35</v>
       </c>
       <c r="L175">
-        <v>9.6001785714285717</v>
+        <v>13.35</v>
       </c>
       <c r="M175">
         <v>12.855178571428571</v>
@@ -10132,7 +10124,7 @@
         <v>11.2</v>
       </c>
       <c r="L176">
-        <v>7.9246428571428567</v>
+        <v>11.2</v>
       </c>
       <c r="M176">
         <v>10.35464285714286</v>
@@ -10182,7 +10174,7 @@
         <v>4</v>
       </c>
       <c r="L177">
-        <v>7.9246428571428567</v>
+        <v>4</v>
       </c>
       <c r="M177">
         <v>10.35464285714286</v>
@@ -10232,7 +10224,7 @@
         <v>6</v>
       </c>
       <c r="L178">
-        <v>17.980535714285711</v>
+        <v>6</v>
       </c>
       <c r="M178">
         <v>20.603035714285721</v>
@@ -10282,7 +10274,7 @@
         <v>9</v>
       </c>
       <c r="L179">
-        <v>7.4394642857142852</v>
+        <v>9</v>
       </c>
       <c r="M179">
         <v>9.663214285714286</v>
@@ -10332,7 +10324,7 @@
         <v>9.4499999999999993</v>
       </c>
       <c r="L180">
-        <v>18.891964285714291</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="M180">
         <v>21.926964285714281</v>
@@ -10382,7 +10374,7 @@
         <v>0</v>
       </c>
       <c r="L181">
-        <v>0</v>
+        <v>7.75</v>
       </c>
       <c r="M181">
         <v>2.2374999999999998</v>
@@ -10432,7 +10424,7 @@
         <v>12.5</v>
       </c>
       <c r="L182">
-        <v>19.34767857142857</v>
+        <v>12.5</v>
       </c>
       <c r="M182">
         <v>22.588928571428571</v>
@@ -10482,7 +10474,7 @@
         <v>8.75</v>
       </c>
       <c r="L183">
-        <v>19.34767857142857</v>
+        <v>8.75</v>
       </c>
       <c r="M183">
         <v>22.588928571428571</v>
@@ -10532,7 +10524,7 @@
         <v>14.15</v>
       </c>
       <c r="L184">
-        <v>18.891964285714291</v>
+        <v>14.15</v>
       </c>
       <c r="M184">
         <v>21.926964285714281</v>
@@ -10582,7 +10574,7 @@
         <v>7</v>
       </c>
       <c r="L185">
-        <v>19.34767857142857</v>
+        <v>7</v>
       </c>
       <c r="M185">
         <v>22.588928571428571</v>
@@ -10632,7 +10624,7 @@
         <v>18.3</v>
       </c>
       <c r="L186">
-        <v>23.21339285714286</v>
+        <v>18.3</v>
       </c>
       <c r="M186">
         <v>24.075892857142861</v>
@@ -10682,7 +10674,7 @@
         <v>13.45</v>
       </c>
       <c r="L187">
-        <v>22.24303571428571</v>
+        <v>13.45</v>
       </c>
       <c r="M187">
         <v>25.896785714285709</v>
@@ -10732,7 +10724,7 @@
         <v>9.5</v>
       </c>
       <c r="L188">
-        <v>7.4689285714285711</v>
+        <v>9.5</v>
       </c>
       <c r="M188">
         <v>9.692678571428571</v>
@@ -10782,7 +10774,7 @@
         <v>16.850000000000001</v>
       </c>
       <c r="L189">
-        <v>21.508392857142859</v>
+        <v>16.850000000000001</v>
       </c>
       <c r="M189">
         <v>23.66339285714286</v>
@@ -10832,7 +10824,7 @@
         <v>15.55</v>
       </c>
       <c r="L190">
-        <v>8.3803571428571431</v>
+        <v>15.55</v>
       </c>
       <c r="M190">
         <v>11.01660714285714</v>
@@ -10882,7 +10874,7 @@
         <v>11.75</v>
       </c>
       <c r="L191">
-        <v>19.80339285714286</v>
+        <v>11.75</v>
       </c>
       <c r="M191">
         <v>23.250892857142858</v>
@@ -10932,7 +10924,7 @@
         <v>8</v>
       </c>
       <c r="L192">
-        <v>8.3803571428571431</v>
+        <v>8</v>
       </c>
       <c r="M192">
         <v>11.01660714285714</v>
@@ -10982,7 +10974,7 @@
         <v>12.6</v>
       </c>
       <c r="L193">
-        <v>23.21339285714286</v>
+        <v>12.6</v>
       </c>
       <c r="M193">
         <v>24.075892857142861</v>
@@ -11032,7 +11024,7 @@
         <v>15.75</v>
       </c>
       <c r="L194">
-        <v>18.436250000000001</v>
+        <v>15.75</v>
       </c>
       <c r="M194">
         <v>21.265000000000001</v>
@@ -11082,7 +11074,7 @@
         <v>0</v>
       </c>
       <c r="L195">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M195">
         <v>3.0625</v>
@@ -11132,7 +11124,7 @@
         <v>13.65</v>
       </c>
       <c r="L196">
-        <v>22.360892857142851</v>
+        <v>13.65</v>
       </c>
       <c r="M196">
         <v>23.86964285714286</v>
@@ -11182,7 +11174,7 @@
         <v>7</v>
       </c>
       <c r="L197">
-        <v>7.4689285714285711</v>
+        <v>7</v>
       </c>
       <c r="M197">
         <v>9.692678571428571</v>
@@ -11232,7 +11224,7 @@
         <v>10</v>
       </c>
       <c r="L198">
-        <v>21.508392857142859</v>
+        <v>10</v>
       </c>
       <c r="M198">
         <v>23.66339285714286</v>
@@ -11282,7 +11274,7 @@
         <v>9</v>
       </c>
       <c r="L199">
-        <v>19.34767857142857</v>
+        <v>9</v>
       </c>
       <c r="M199">
         <v>22.588928571428571</v>
@@ -11332,7 +11324,7 @@
         <v>3</v>
       </c>
       <c r="L200">
-        <v>7.4689285714285711</v>
+        <v>3</v>
       </c>
       <c r="M200">
         <v>9.692678571428571</v>
@@ -11382,7 +11374,7 @@
         <v>10.25</v>
       </c>
       <c r="L201">
-        <v>17.980535714285711</v>
+        <v>10.25</v>
       </c>
       <c r="M201">
         <v>20.603035714285721</v>
@@ -11432,7 +11424,7 @@
         <v>12.55</v>
       </c>
       <c r="L202">
-        <v>19.80339285714286</v>
+        <v>12.55</v>
       </c>
       <c r="M202">
         <v>23.250892857142858</v>
@@ -11482,7 +11474,7 @@
         <v>11.7</v>
       </c>
       <c r="L203">
-        <v>19.80339285714286</v>
+        <v>11.7</v>
       </c>
       <c r="M203">
         <v>23.250892857142858</v>
@@ -11532,7 +11524,7 @@
         <v>14.7</v>
       </c>
       <c r="L204">
-        <v>23.21339285714286</v>
+        <v>14.7</v>
       </c>
       <c r="M204">
         <v>24.075892857142861</v>
@@ -11582,7 +11574,7 @@
         <v>0</v>
       </c>
       <c r="L205">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M205">
         <v>2.2374999999999998</v>
@@ -11632,7 +11624,7 @@
         <v>0</v>
       </c>
       <c r="L206">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M206">
         <v>2.2374999999999998</v>
@@ -11682,7 +11674,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="L207">
-        <v>18.436250000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="M207">
         <v>21.265000000000001</v>
@@ -11732,7 +11724,7 @@
         <v>10</v>
       </c>
       <c r="L208">
-        <v>19.34767857142857</v>
+        <v>10</v>
       </c>
       <c r="M208">
         <v>22.588928571428571</v>
@@ -11782,7 +11774,7 @@
         <v>5</v>
       </c>
       <c r="L209">
-        <v>8.3803571428571431</v>
+        <v>5</v>
       </c>
       <c r="M209">
         <v>11.01660714285714</v>
@@ -11832,7 +11824,7 @@
         <v>15.8</v>
       </c>
       <c r="L210">
-        <v>20.655892857142859</v>
+        <v>15.8</v>
       </c>
       <c r="M210">
         <v>23.457142857142859</v>
@@ -11882,7 +11874,7 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="L211">
-        <v>18.891964285714291</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="M211">
         <v>21.926964285714281</v>
@@ -11932,7 +11924,7 @@
         <v>0</v>
       </c>
       <c r="L212">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M212">
         <v>2.2374999999999998</v>
@@ -11982,7 +11974,7 @@
         <v>13.1</v>
       </c>
       <c r="L213">
-        <v>17.980535714285711</v>
+        <v>13.1</v>
       </c>
       <c r="M213">
         <v>20.603035714285721</v>
@@ -12032,7 +12024,7 @@
         <v>12.9</v>
       </c>
       <c r="L214">
-        <v>19.34767857142857</v>
+        <v>12.9</v>
       </c>
       <c r="M214">
         <v>22.588928571428571</v>
@@ -12082,7 +12074,7 @@
         <v>12</v>
       </c>
       <c r="L215">
-        <v>18.891964285714291</v>
+        <v>12</v>
       </c>
       <c r="M215">
         <v>21.926964285714281</v>
@@ -12132,7 +12124,7 @@
         <v>11.25</v>
       </c>
       <c r="L216">
-        <v>18.436250000000001</v>
+        <v>11.25</v>
       </c>
       <c r="M216">
         <v>21.265000000000001</v>
@@ -12182,7 +12174,7 @@
         <v>16.350000000000001</v>
       </c>
       <c r="L217">
-        <v>7.4689285714285711</v>
+        <v>16.350000000000001</v>
       </c>
       <c r="M217">
         <v>9.692678571428571</v>
@@ -12232,7 +12224,7 @@
         <v>11.65</v>
       </c>
       <c r="L218">
-        <v>18.436250000000001</v>
+        <v>11.65</v>
       </c>
       <c r="M218">
         <v>21.265000000000001</v>
@@ -12282,7 +12274,7 @@
         <v>0</v>
       </c>
       <c r="L219">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="M219">
         <v>2.2374999999999998</v>
@@ -12332,7 +12324,7 @@
         <v>12.55</v>
       </c>
       <c r="L220">
-        <v>8.3803571428571431</v>
+        <v>12.55</v>
       </c>
       <c r="M220">
         <v>11.01660714285714</v>
@@ -12382,7 +12374,7 @@
         <v>19.2</v>
       </c>
       <c r="L221">
-        <v>7.9246428571428567</v>
+        <v>19.2</v>
       </c>
       <c r="M221">
         <v>10.35464285714286</v>
@@ -12432,7 +12424,7 @@
         <v>8.75</v>
       </c>
       <c r="L222">
-        <v>21.508392857142859</v>
+        <v>8.75</v>
       </c>
       <c r="M222">
         <v>23.66339285714286</v>
@@ -12482,7 +12474,7 @@
         <v>14.85</v>
       </c>
       <c r="L223">
-        <v>20.655892857142859</v>
+        <v>14.85</v>
       </c>
       <c r="M223">
         <v>23.457142857142859</v>
@@ -12532,7 +12524,7 @@
         <v>16.5</v>
       </c>
       <c r="L224">
-        <v>8.3803571428571431</v>
+        <v>16.5</v>
       </c>
       <c r="M224">
         <v>11.01660714285714</v>
@@ -12582,7 +12574,7 @@
         <v>16</v>
       </c>
       <c r="L225">
-        <v>23.21339285714286</v>
+        <v>16</v>
       </c>
       <c r="M225">
         <v>24.92839285714286</v>
@@ -12632,7 +12624,7 @@
         <v>12.9</v>
       </c>
       <c r="L226">
-        <v>7.4689285714285711</v>
+        <v>12.9</v>
       </c>
       <c r="M226">
         <v>9.692678571428571</v>
@@ -12682,7 +12674,7 @@
         <v>11</v>
       </c>
       <c r="L227">
-        <v>7.0132142857142856</v>
+        <v>11</v>
       </c>
       <c r="M227">
         <v>9.0307142857142857</v>
@@ -12732,7 +12724,7 @@
         <v>9.25</v>
       </c>
       <c r="L228">
-        <v>21.508392857142859</v>
+        <v>9.25</v>
       </c>
       <c r="M228">
         <v>25.368392857142862</v>
@@ -12782,7 +12774,7 @@
         <v>8.0500000000000007</v>
       </c>
       <c r="L229">
-        <v>20.655892857142859</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="M229">
         <v>23.457142857142859</v>
@@ -12832,7 +12824,7 @@
         <v>11</v>
       </c>
       <c r="L230">
-        <v>8.8360714285714295</v>
+        <v>11</v>
       </c>
       <c r="M230">
         <v>11.678571428571431</v>
@@ -12882,7 +12874,7 @@
         <v>5</v>
       </c>
       <c r="L231">
-        <v>8.3803571428571431</v>
+        <v>18.7</v>
       </c>
       <c r="M231">
         <v>11.01660714285714</v>
@@ -12932,7 +12924,7 @@
         <v>12.6</v>
       </c>
       <c r="L232">
-        <v>19.80339285714286</v>
+        <v>12.6</v>
       </c>
       <c r="M232">
         <v>23.250892857142858</v>
@@ -12982,7 +12974,7 @@
         <v>11.9</v>
       </c>
       <c r="L233">
-        <v>20.655892857142859</v>
+        <v>11.9</v>
       </c>
       <c r="M233">
         <v>23.457142857142859</v>
@@ -13032,7 +13024,7 @@
         <v>7.75</v>
       </c>
       <c r="L234">
-        <v>17.980535714285711</v>
+        <v>7.75</v>
       </c>
       <c r="M234">
         <v>20.603035714285721</v>
@@ -13082,7 +13074,7 @@
         <v>12.45</v>
       </c>
       <c r="L235">
-        <v>19.80339285714286</v>
+        <v>12.45</v>
       </c>
       <c r="M235">
         <v>23.250892857142858</v>
@@ -13132,7 +13124,7 @@
         <v>5</v>
       </c>
       <c r="L236">
-        <v>8.8360714285714295</v>
+        <v>5</v>
       </c>
       <c r="M236">
         <v>11.678571428571431</v>
@@ -13182,7 +13174,7 @@
         <v>14.2</v>
       </c>
       <c r="L237">
-        <v>19.80339285714286</v>
+        <v>14.2</v>
       </c>
       <c r="M237">
         <v>23.250892857142858</v>
@@ -13232,7 +13224,7 @@
         <v>11.55</v>
       </c>
       <c r="L238">
-        <v>18.436250000000001</v>
+        <v>11.55</v>
       </c>
       <c r="M238">
         <v>21.265000000000001</v>
@@ -13282,7 +13274,7 @@
         <v>14.7</v>
       </c>
       <c r="L239">
-        <v>23.21339285714286</v>
+        <v>14.7</v>
       </c>
       <c r="M239">
         <v>24.075892857142861</v>
@@ -13332,7 +13324,7 @@
         <v>11.7</v>
       </c>
       <c r="L240">
-        <v>7.9246428571428567</v>
+        <v>11.7</v>
       </c>
       <c r="M240">
         <v>10.35464285714286</v>
@@ -13382,7 +13374,7 @@
         <v>11.9</v>
       </c>
       <c r="L241">
-        <v>7.4689285714285711</v>
+        <v>11.9</v>
       </c>
       <c r="M241">
         <v>9.692678571428571</v>
@@ -13432,7 +13424,7 @@
         <v>5</v>
       </c>
       <c r="L242">
-        <v>18.436250000000001</v>
+        <v>5</v>
       </c>
       <c r="M242">
         <v>21.265000000000001</v>
@@ -13482,7 +13474,7 @@
         <v>5</v>
       </c>
       <c r="L243">
-        <v>7.0132142857142856</v>
+        <v>5</v>
       </c>
       <c r="M243">
         <v>9.0307142857142857</v>
@@ -13532,7 +13524,7 @@
         <v>9.1</v>
       </c>
       <c r="L244">
-        <v>20.655892857142859</v>
+        <v>9.1</v>
       </c>
       <c r="M244">
         <v>23.457142857142859</v>
@@ -13582,7 +13574,7 @@
         <v>13</v>
       </c>
       <c r="L245">
-        <v>18.891964285714291</v>
+        <v>13</v>
       </c>
       <c r="M245">
         <v>21.926964285714281</v>
@@ -13632,7 +13624,7 @@
         <v>13.75</v>
       </c>
       <c r="L246">
-        <v>18.891964285714291</v>
+        <v>13.75</v>
       </c>
       <c r="M246">
         <v>21.926964285714281</v>
@@ -13682,7 +13674,7 @@
         <v>10</v>
       </c>
       <c r="L247">
-        <v>19.80339285714286</v>
+        <v>10</v>
       </c>
       <c r="M247">
         <v>23.250892857142858</v>
@@ -13732,7 +13724,7 @@
         <v>8.25</v>
       </c>
       <c r="L248">
-        <v>19.34767857142857</v>
+        <v>8.25</v>
       </c>
       <c r="M248">
         <v>22.588928571428571</v>
@@ -13782,7 +13774,7 @@
         <v>13.5</v>
       </c>
       <c r="L249">
-        <v>18.436250000000001</v>
+        <v>13.5</v>
       </c>
       <c r="M249">
         <v>21.265000000000001</v>
@@ -13832,7 +13824,7 @@
         <v>14.65</v>
       </c>
       <c r="L250">
-        <v>7.4689285714285711</v>
+        <v>14.65</v>
       </c>
       <c r="M250">
         <v>9.692678571428571</v>
@@ -13882,7 +13874,7 @@
         <v>0</v>
       </c>
       <c r="L251">
-        <v>0</v>
+        <v>13.25</v>
       </c>
       <c r="M251">
         <v>2.4437500000000001</v>
@@ -13932,7 +13924,7 @@
         <v>10.050000000000001</v>
       </c>
       <c r="L252">
-        <v>20.596964285714289</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="M252">
         <v>24.044464285714291</v>
@@ -13982,7 +13974,7 @@
         <v>5.5</v>
       </c>
       <c r="L253">
-        <v>17.980535714285711</v>
+        <v>5.5</v>
       </c>
       <c r="M253">
         <v>20.603035714285721</v>
@@ -14032,7 +14024,7 @@
         <v>11.55</v>
       </c>
       <c r="L254">
-        <v>17.980535714285711</v>
+        <v>11.55</v>
       </c>
       <c r="M254">
         <v>20.603035714285721</v>
@@ -14082,7 +14074,7 @@
         <v>10.95</v>
       </c>
       <c r="L255">
-        <v>21.508392857142859</v>
+        <v>10.95</v>
       </c>
       <c r="M255">
         <v>23.66339285714286</v>
@@ -14132,7 +14124,7 @@
         <v>13.5</v>
       </c>
       <c r="L256">
-        <v>20.655892857142859</v>
+        <v>13.5</v>
       </c>
       <c r="M256">
         <v>23.457142857142859</v>
@@ -14182,7 +14174,7 @@
         <v>0</v>
       </c>
       <c r="L257">
-        <v>0</v>
+        <v>12.25</v>
       </c>
       <c r="M257">
         <v>2.2374999999999998</v>
@@ -14232,7 +14224,7 @@
         <v>12.8</v>
       </c>
       <c r="L258">
-        <v>20.655892857142859</v>
+        <v>12.8</v>
       </c>
       <c r="M258">
         <v>23.457142857142859</v>
@@ -14282,7 +14274,7 @@
         <v>11.85</v>
       </c>
       <c r="L259">
-        <v>8.8066071428571426</v>
+        <v>11.85</v>
       </c>
       <c r="M259">
         <v>11.64910714285714</v>
@@ -14332,7 +14324,7 @@
         <v>11.9</v>
       </c>
       <c r="L260">
-        <v>19.80339285714286</v>
+        <v>11.9</v>
       </c>
       <c r="M260">
         <v>23.250892857142858</v>
@@ -14382,7 +14374,7 @@
         <v>13.85</v>
       </c>
       <c r="L261">
-        <v>23.21339285714286</v>
+        <v>13.85</v>
       </c>
       <c r="M261">
         <v>24.075892857142861</v>
@@ -14432,7 +14424,7 @@
         <v>6</v>
       </c>
       <c r="L262">
-        <v>20.655892857142859</v>
+        <v>6</v>
       </c>
       <c r="M262">
         <v>23.457142857142859</v>
@@ -14482,7 +14474,7 @@
         <v>7.25</v>
       </c>
       <c r="L263">
-        <v>7.0132142857142856</v>
+        <v>7.25</v>
       </c>
       <c r="M263">
         <v>9.0307142857142857</v>
@@ -14532,7 +14524,7 @@
         <v>13.5</v>
       </c>
       <c r="L264">
-        <v>19.80339285714286</v>
+        <v>13.5</v>
       </c>
       <c r="M264">
         <v>23.250892857142858</v>
@@ -14582,7 +14574,7 @@
         <v>6</v>
       </c>
       <c r="L265">
-        <v>8.8360714285714295</v>
+        <v>6</v>
       </c>
       <c r="M265">
         <v>11.678571428571431</v>
@@ -14632,7 +14624,7 @@
         <v>12.3</v>
       </c>
       <c r="L266">
-        <v>18.891964285714291</v>
+        <v>12.3</v>
       </c>
       <c r="M266">
         <v>21.926964285714281</v>
@@ -14682,7 +14674,7 @@
         <v>10.85</v>
       </c>
       <c r="L267">
-        <v>23.21339285714286</v>
+        <v>10.85</v>
       </c>
       <c r="M267">
         <v>24.075892857142861</v>
@@ -14732,7 +14724,7 @@
         <v>0</v>
       </c>
       <c r="L268">
-        <v>0</v>
+        <v>13.9</v>
       </c>
       <c r="M268">
         <v>2.2374999999999998</v>
@@ -14782,7 +14774,7 @@
         <v>6</v>
       </c>
       <c r="L269">
-        <v>8.8360714285714295</v>
+        <v>6</v>
       </c>
       <c r="M269">
         <v>11.678571428571431</v>
@@ -14832,7 +14824,7 @@
         <v>4</v>
       </c>
       <c r="L270">
-        <v>7.4689285714285711</v>
+        <v>4</v>
       </c>
       <c r="M270">
         <v>9.692678571428571</v>
@@ -14882,7 +14874,7 @@
         <v>9.25</v>
       </c>
       <c r="L271">
-        <v>23.21339285714286</v>
+        <v>9.25</v>
       </c>
       <c r="M271">
         <v>24.92839285714286</v>
@@ -14932,7 +14924,7 @@
         <v>0</v>
       </c>
       <c r="L272">
-        <v>0</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="M272">
         <v>2.2374999999999998</v>
@@ -14982,7 +14974,7 @@
         <v>12.3</v>
       </c>
       <c r="L273">
-        <v>7.4689285714285711</v>
+        <v>12.3</v>
       </c>
       <c r="M273">
         <v>9.692678571428571</v>
@@ -15032,7 +15024,7 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="L274">
-        <v>18.891964285714291</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="M274">
         <v>21.926964285714281</v>
@@ -15082,7 +15074,7 @@
         <v>10.65</v>
       </c>
       <c r="L275">
-        <v>8.3508928571428562</v>
+        <v>10.65</v>
       </c>
       <c r="M275">
         <v>10.98714285714286</v>
@@ -15132,7 +15124,7 @@
         <v>11</v>
       </c>
       <c r="L276">
-        <v>19.34767857142857</v>
+        <v>11</v>
       </c>
       <c r="M276">
         <v>22.588928571428571</v>
@@ -15182,7 +15174,7 @@
         <v>11.8</v>
       </c>
       <c r="L277">
-        <v>7.0132142857142856</v>
+        <v>11.8</v>
       </c>
       <c r="M277">
         <v>9.0307142857142857</v>
@@ -15232,7 +15224,7 @@
         <v>6</v>
       </c>
       <c r="L278">
-        <v>8.3803571428571431</v>
+        <v>6</v>
       </c>
       <c r="M278">
         <v>11.01660714285714</v>
@@ -15282,7 +15274,7 @@
         <v>4</v>
       </c>
       <c r="L279">
-        <v>7.0132142857142856</v>
+        <v>14.55</v>
       </c>
       <c r="M279">
         <v>9.0307142857142857</v>
@@ -15332,7 +15324,7 @@
         <v>12.75</v>
       </c>
       <c r="L280">
-        <v>22.360892857142851</v>
+        <v>12.75</v>
       </c>
       <c r="M280">
         <v>23.86964285714286</v>
@@ -15382,7 +15374,7 @@
         <v>15.1</v>
       </c>
       <c r="L281">
-        <v>18.436250000000001</v>
+        <v>15.1</v>
       </c>
       <c r="M281">
         <v>21.265000000000001</v>
@@ -15432,7 +15424,7 @@
         <v>9.4499999999999993</v>
       </c>
       <c r="L282">
-        <v>20.655892857142859</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="M282">
         <v>23.457142857142859</v>
@@ -15482,7 +15474,7 @@
         <v>8.5</v>
       </c>
       <c r="L283">
-        <v>8.3803571428571431</v>
+        <v>8.5</v>
       </c>
       <c r="M283">
         <v>11.01660714285714</v>
@@ -15532,7 +15524,7 @@
         <v>0</v>
       </c>
       <c r="L284">
-        <v>0</v>
+        <v>11.55</v>
       </c>
       <c r="M284">
         <v>2.2374999999999998</v>
@@ -15582,7 +15574,7 @@
         <v>12.9</v>
       </c>
       <c r="L285">
-        <v>18.891964285714291</v>
+        <v>12.9</v>
       </c>
       <c r="M285">
         <v>21.926964285714281</v>
@@ -15632,7 +15624,7 @@
         <v>8</v>
       </c>
       <c r="L286">
-        <v>7.4689285714285711</v>
+        <v>8</v>
       </c>
       <c r="M286">
         <v>9.692678571428571</v>
@@ -15682,7 +15674,7 @@
         <v>10.85</v>
       </c>
       <c r="L287">
-        <v>7.9246428571428567</v>
+        <v>10.85</v>
       </c>
       <c r="M287">
         <v>10.35464285714286</v>
@@ -15732,7 +15724,7 @@
         <v>6</v>
       </c>
       <c r="L288">
-        <v>17.980535714285711</v>
+        <v>6</v>
       </c>
       <c r="M288">
         <v>20.603035714285721</v>
@@ -15782,7 +15774,7 @@
         <v>13.45</v>
       </c>
       <c r="L289">
-        <v>19.34767857142857</v>
+        <v>13.45</v>
       </c>
       <c r="M289">
         <v>22.588928571428571</v>
@@ -15832,7 +15824,7 @@
         <v>15.05</v>
       </c>
       <c r="L290">
-        <v>20.655892857142859</v>
+        <v>15.05</v>
       </c>
       <c r="M290">
         <v>23.457142857142859</v>
@@ -15882,7 +15874,7 @@
         <v>5</v>
       </c>
       <c r="L291">
-        <v>7.4689285714285711</v>
+        <v>16.45</v>
       </c>
       <c r="M291">
         <v>9.692678571428571</v>
@@ -15932,7 +15924,7 @@
         <v>8.4</v>
       </c>
       <c r="L292">
-        <v>20.655892857142859</v>
+        <v>8.4</v>
       </c>
       <c r="M292">
         <v>23.457142857142859</v>
@@ -15982,7 +15974,7 @@
         <v>8.25</v>
       </c>
       <c r="L293">
-        <v>7.9246428571428567</v>
+        <v>8.25</v>
       </c>
       <c r="M293">
         <v>10.35464285714286</v>
@@ -16032,7 +16024,7 @@
         <v>12.55</v>
       </c>
       <c r="L294">
-        <v>8.3803571428571431</v>
+        <v>12.55</v>
       </c>
       <c r="M294">
         <v>11.01660714285714</v>
@@ -16082,7 +16074,7 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="L295">
-        <v>8.8360714285714295</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="M295">
         <v>11.678571428571431</v>
@@ -16132,7 +16124,7 @@
         <v>8.75</v>
       </c>
       <c r="L296">
-        <v>8.8360714285714295</v>
+        <v>8.75</v>
       </c>
       <c r="M296">
         <v>11.678571428571431</v>
@@ -16182,7 +16174,7 @@
         <v>13.8</v>
       </c>
       <c r="L297">
-        <v>23.21339285714286</v>
+        <v>13.8</v>
       </c>
       <c r="M297">
         <v>24.075892857142861</v>
@@ -16232,7 +16224,7 @@
         <v>12.1</v>
       </c>
       <c r="L298">
-        <v>20.655892857142859</v>
+        <v>12.1</v>
       </c>
       <c r="M298">
         <v>23.457142857142859</v>
@@ -16282,7 +16274,7 @@
         <v>7</v>
       </c>
       <c r="L299">
-        <v>23.21339285714286</v>
+        <v>7</v>
       </c>
       <c r="M299">
         <v>24.075892857142861</v>
@@ -16332,7 +16324,7 @@
         <v>8.0500000000000007</v>
       </c>
       <c r="L300">
-        <v>18.891964285714291</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="M300">
         <v>21.926964285714281</v>
@@ -16382,7 +16374,7 @@
         <v>0</v>
       </c>
       <c r="L301">
-        <v>0</v>
+        <v>15.35</v>
       </c>
       <c r="M301">
         <v>2.2374999999999998</v>
@@ -16432,7 +16424,7 @@
         <v>0</v>
       </c>
       <c r="L302">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="M302">
         <v>2.2374999999999998</v>

</xml_diff>